<commit_message>
fixed bugs in the codes
</commit_message>
<xml_diff>
--- a/mcmaster_excel/Fine-Thread_Metric_316_Stainless_Steel_Button
______Head_Hex_Drive_Screws.xlsx
+++ b/mcmaster_excel/Fine-Thread_Metric_316_Stainless_Steel_Button
______Head_Hex_Drive_Screws.xlsx
@@ -481,27 +481,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HeadDia., mm</t>
+          <t>Head Dia., mm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>HeadHt., mm</t>
+          <t>Head Ht., mm</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DriveSize, mm</t>
+          <t>Drive Size, mm</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>TensileStrength, psi</t>
+          <t>Tensile Strength, psi</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SpecificationsMet</t>
+          <t>Specifications Met</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>

</xml_diff>